<commit_message>
vault backup: 2024-11-05 11:22:26
</commit_message>
<xml_diff>
--- a/2024-2/Evaluación de proyectos/Excels/C3_Cáceres_Iván.xlsx
+++ b/2024-2/Evaluación de proyectos/Excels/C3_Cáceres_Iván.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivaaan\Desktop\git\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3A35A4-09B0-459F-9998-BA56B1E37972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA98AC-2613-4326-B132-9D8D0939C3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5B8BD1F-5DE6-414C-9A7D-5B960CA65C48}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
-  <si>
-    <t>?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Ri</t>
   </si>
@@ -65,9 +62,6 @@
     <t>VARIANZA</t>
   </si>
   <si>
-    <t>ESTADO FINANCIERO ?</t>
-  </si>
-  <si>
     <t>EMPRESAS QUE COMPONEN LA INDUSTRIA DE ?</t>
   </si>
   <si>
@@ -138,6 +132,27 @@
   </si>
   <si>
     <t>Iván Andrés Cáceres Satorres</t>
+  </si>
+  <si>
+    <t>COPEC</t>
+  </si>
+  <si>
+    <t>ESTADO FINANCIERO EPERVA</t>
+  </si>
+  <si>
+    <t>LLOYD</t>
+  </si>
+  <si>
+    <t>PUERTO MONTT</t>
+  </si>
+  <si>
+    <t>PESQUERA NILALHUE</t>
+  </si>
+  <si>
+    <t>CELCO</t>
+  </si>
+  <si>
+    <t>EPERVA</t>
   </si>
 </sst>
 </file>
@@ -147,7 +162,7 @@
   <numFmts count="1">
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,13 +185,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -217,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,15 +254,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,7 +267,22 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,179 +624,190 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="A1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="8" t="str">
+        <f>A2</f>
+        <v>COPEC</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="4" t="str">
-        <f>A2</f>
-        <v>?</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <f>_xlfn.COVARIANCE.P(B5:B11,C5:C11)</f>
+        <v>3.3673469387755089E-4</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="e">
-        <f>_xlfn.COVARIANCE.P(B5:B11,C5:C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="2" t="e">
+      <c r="H3" s="9">
         <f>F3/F4</f>
-        <v>#DIV/0!</v>
+        <v>0.29963680387409108</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="str">
         <f>A2</f>
-        <v>?</v>
+        <v>COPEC</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5" t="e">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2">
         <f>_xlfn.VAR.S(C5:C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="2"/>
+        <v>1.1238095238095269E-3</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="2">
         <v>2013</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>0</v>
+      <c r="B5" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.09</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="2">
         <v>2014</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>0</v>
+      <c r="B6" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.08</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="2">
         <v>2015</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>0</v>
+      <c r="B7" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.12</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="2">
         <v>2016</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>0</v>
+      <c r="B8" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.13</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="2">
         <v>2017</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>0</v>
+      <c r="B9" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.15</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="2">
         <v>2018</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>0</v>
+      <c r="B10" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.1</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="2">
         <v>2019</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>0</v>
+      <c r="B11" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.05</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -778,149 +822,149 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="4" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="1"/>
       <c r="F14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="4">
+        <v>16500</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3800</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H15" s="4">
+        <v>5300</v>
+      </c>
+      <c r="I15" s="4">
+        <v>4000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B16" s="4">
+        <v>300</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3900</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="H16" s="4">
+        <v>7000</v>
+      </c>
+      <c r="I16" s="4">
+        <v>3500</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="B17" s="4">
+        <v>3200</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="D17" s="4">
+        <v>12300</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="H17" s="4">
+        <v>6000</v>
+      </c>
+      <c r="I17" s="4">
+        <v>4000</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="8">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5">
         <f>SUM(B15:B17)</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="8">
+        <v>20</v>
+      </c>
+      <c r="D18" s="5">
         <f>SUM(D15:D17)</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="5" t="e">
+        <v>21</v>
+      </c>
+      <c r="G18" s="2">
         <f>AVERAGE(G15:G17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -930,23 +974,23 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="7">
+        <v>20</v>
+      </c>
+      <c r="H19" s="4">
         <f>SUM(H15:H17)</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="7">
+        <v>18300</v>
+      </c>
+      <c r="I19" s="4">
         <f>SUM(I15:I17)</f>
-        <v>0</v>
+        <v>11500</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.25</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -955,10 +999,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.02</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -967,10 +1011,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.13</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -979,11 +1023,11 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="9" t="e">
+        <v>24</v>
+      </c>
+      <c r="B23" s="6">
         <f>B22-B21</f>
-        <v>#VALUE!</v>
+        <v>0.11</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -992,10 +1036,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="B24" s="6">
+        <v>7.8E-2</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1011,173 +1055,173 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
+      <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="I26" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="7" t="e">
+        <v>32</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3845</v>
+      </c>
+      <c r="C27" s="4">
+        <v>17980</v>
+      </c>
+      <c r="D27" s="4">
         <f>B27+C27</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E27" s="5" t="e">
+        <v>21825</v>
+      </c>
+      <c r="E27" s="2">
         <f>D27/D30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F27" s="5" t="e">
+        <v>0.26785714285714285</v>
+      </c>
+      <c r="F27" s="2">
         <f>H3/(1+(1-B20)*(B27/C27))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G27" s="5" t="e">
+        <v>0.25822154376160361</v>
+      </c>
+      <c r="G27" s="2">
         <f>H3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H27" s="5" t="e">
+        <v>0.29963680387409108</v>
+      </c>
+      <c r="H27" s="7">
         <f>B21+G27*B23</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I27" s="10" t="e">
+        <v>5.2960048426150014E-2</v>
+      </c>
+      <c r="I27" s="7">
         <f>(B27/D27)*(1-B20)*B24+(C27/D27)*H27</f>
-        <v>#VALUE!</v>
+        <v>5.3936044476617512E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="7" t="e">
+        <v>37</v>
+      </c>
+      <c r="B28" s="4">
+        <v>3975</v>
+      </c>
+      <c r="C28" s="4">
+        <v>35680</v>
+      </c>
+      <c r="D28" s="4">
         <f t="shared" ref="D28:D30" si="0">B28+C28</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E28" s="5" t="e">
+        <v>39655</v>
+      </c>
+      <c r="E28" s="2">
         <f>D28/D30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="5" t="e">
-        <f>F28*(1+(1-B20)*(B28/C28))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H28" s="5" t="e">
+        <v>0.48668384879725085</v>
+      </c>
+      <c r="F28" s="2">
+        <f>G28/(1+(1-B20)*(B28/C28))</f>
+        <v>1.7904025348378543</v>
+      </c>
+      <c r="G28" s="11">
+        <v>1.94</v>
+      </c>
+      <c r="H28" s="7">
         <f>B21+G28*B23</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I28" s="10" t="e">
+        <v>0.2334</v>
+      </c>
+      <c r="I28" s="7">
         <f>(B28/D28)*(1-B20)*B24+(C28/D28)*H28</f>
-        <v>#VALUE!</v>
+        <v>0.21586809986130373</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="7">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4">
         <f>SUM(D15:D16)</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="7" t="str">
+        <v>7700</v>
+      </c>
+      <c r="C29" s="4">
         <f>D17</f>
-        <v>?</v>
-      </c>
-      <c r="D29" s="7" t="e">
+        <v>12300</v>
+      </c>
+      <c r="D29" s="4">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E29" s="5" t="e">
+        <v>20000</v>
+      </c>
+      <c r="E29" s="2">
         <f>D29/D30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F29" s="5" t="e">
+        <v>0.24545900834560627</v>
+      </c>
+      <c r="F29" s="2">
         <f>G18/(1+(1-B20)*(H19/I19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G29" s="5" t="e">
+        <v>0.72943508424182368</v>
+      </c>
+      <c r="G29" s="2">
         <f>F29*(1+(1-B20)*(B29/C29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H29" s="5" t="e">
+        <v>1.0719137518431676</v>
+      </c>
+      <c r="H29" s="7">
         <f>B21+G29*B23</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I29" s="10" t="e">
+        <v>0.13791051270274843</v>
+      </c>
+      <c r="I29" s="7">
         <f>(B29/D29)*(1-B20)*B24+(C29/D29)*H29</f>
-        <v>#VALUE!</v>
+        <v>0.10733746531219028</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="7">
+        <v>30</v>
+      </c>
+      <c r="B30" s="4">
         <f>SUM(B27:B29)</f>
-        <v>0</v>
-      </c>
-      <c r="C30" s="7">
+        <v>15520</v>
+      </c>
+      <c r="C30" s="4">
         <f>SUM(C27:C29)</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="7">
+        <v>65960</v>
+      </c>
+      <c r="D30" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="5" t="e">
+        <v>81480</v>
+      </c>
+      <c r="E30" s="2">
         <f>D30/D30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F30" s="5" t="e">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
         <f>F27*E27+F28*E28+F29*E29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G30" s="5" t="e">
+        <v>1.1195728939178766</v>
+      </c>
+      <c r="G30" s="2">
         <f>F30*(1+(1-B20)*(B30/C30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H30" s="5" t="e">
+        <v>1.317144581079855</v>
+      </c>
+      <c r="H30" s="7">
         <f>B21+G30*B23</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I30" s="10" t="e">
+        <v>0.16488590391878405</v>
+      </c>
+      <c r="I30" s="7">
         <f>(B30/D30)*(1-B20)*B24+(C30/D30)*H30</f>
-        <v>#DIV/0!</v>
+        <v>0.14462192221996806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>